<commit_message>
removal of unneeded garbage collection
</commit_message>
<xml_diff>
--- a/AlgorithmSpeeds.xlsx
+++ b/AlgorithmSpeeds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding_Projects\Python\Mirage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EC4A65-967F-4E8A-BC75-1C19F10CFDE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A882B1-47F5-4173-A42F-ADB407640275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15960" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t>Algorithm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Average Time Taken In Seconds</t>
   </si>
@@ -45,9 +42,6 @@
     <t>Without Print Statements</t>
   </si>
   <si>
-    <t>Notes: The garbage thread collection could also be holding back the speed. Might want to try optimizing this.</t>
-  </si>
-  <si>
     <t>Start File Directory and rough file count</t>
   </si>
   <si>
@@ -60,17 +54,38 @@
     <t>Note: This might make the checking a little unstable as the threads are less controlled as to when the function is finished</t>
   </si>
   <si>
-    <t>History_Compare()</t>
-  </si>
-  <si>
     <t>Generate_Hash()</t>
+  </si>
+  <si>
+    <t>Check_File_Data()</t>
+  </si>
+  <si>
+    <t>Ran in WSL2</t>
+  </si>
+  <si>
+    <t>Ran in Windows10 (Pycharm)</t>
+  </si>
+  <si>
+    <t>Why does it run so much slower in WSL2? Would it run faster on actual hardware (no VM)?</t>
+  </si>
+  <si>
+    <t>The garbage thread collection could also be holding back the speed. Might want to try optimizing this.</t>
+  </si>
+  <si>
+    <t>Algorithm/What Changed</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Comparison between runtimes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +107,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +132,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -119,21 +146,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -141,11 +190,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -423,49 +497,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.36328125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.453125" customWidth="1"/>
     <col min="6" max="6" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="51.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>91.333334299900002</v>
@@ -476,18 +554,21 @@
       <c r="E2">
         <v>91.082848499999997</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>AVERAGE(C2, D2, E2)</f>
         <v>90.865427499966657</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="G2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -498,115 +579,191 @@
       <c r="E3">
         <v>65.114393299999307</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>AVERAGE(C3,D3,E3)</f>
         <v>64.197425433332938</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
         <v>72.1330758</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>73.411726299999998</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>74.018457398999999</v>
-      </c>
-      <c r="F5" s="6">
-        <f>AVERAGE(C5, D5, E5)</f>
-        <v>73.187753166333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>45.85132669</v>
-      </c>
-      <c r="D6">
-        <v>46.321259300000001</v>
-      </c>
-      <c r="E6">
-        <v>46.554423199989998</v>
       </c>
       <c r="F6" s="5">
         <f>AVERAGE(C6, D6, E6)</f>
+        <v>73.187753166333337</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>45.85132669</v>
+      </c>
+      <c r="D7">
+        <v>46.321259300000001</v>
+      </c>
+      <c r="E7">
+        <v>46.554423199989998</v>
+      </c>
+      <c r="F7" s="4">
+        <f>AVERAGE(C7, D7, E7)</f>
         <v>46.242336396663326</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
+      <c r="C10">
+        <v>49.129974398999998</v>
+      </c>
+      <c r="D10">
+        <v>49.583049000000003</v>
+      </c>
+      <c r="E10">
+        <v>51.894441799900001</v>
+      </c>
+      <c r="F10" s="5">
+        <f>AVERAGE(C10, D10, E10)</f>
+        <v>50.202488399633332</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" t="s">
+      <c r="C11">
+        <v>36.796308599900001</v>
+      </c>
+      <c r="D11">
+        <v>39.372874699999997</v>
+      </c>
+      <c r="E11">
+        <v>40.202507998999998</v>
+      </c>
+      <c r="F11" s="4">
+        <f>AVERAGE(C11, D11, E11)</f>
+        <v>38.790563766300004</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>7.8203649999999998</v>
+      </c>
+      <c r="D13">
+        <v>12.862031699999999</v>
+      </c>
+      <c r="E13">
+        <v>12.167046499</v>
+      </c>
+      <c r="F13" s="4">
+        <f>AVERAGE(C13, D13, E13)</f>
+        <v>10.949814399666666</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>49.129974398999998</v>
-      </c>
-      <c r="D8">
-        <v>49.583049000000003</v>
-      </c>
-      <c r="E8">
-        <v>51.894441799900001</v>
-      </c>
-      <c r="F8" s="6">
-        <f>AVERAGE(C8, D8, E8)</f>
-        <v>50.202488399633332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s">
+    </row>
+    <row r="14" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14">
+        <v>38.194091299</v>
+      </c>
+      <c r="D14">
+        <v>36.855553200000003</v>
+      </c>
+      <c r="E14">
+        <v>38.246856698999999</v>
+      </c>
+      <c r="F14" s="5">
+        <f>AVERAGE(C14, D14, E14)</f>
+        <v>37.765500399333341</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>36.796308599900001</v>
-      </c>
-      <c r="D9">
-        <v>39.372874699999997</v>
-      </c>
-      <c r="E9">
-        <v>40.202507998999998</v>
-      </c>
-      <c r="F9" s="5">
-        <f>AVERAGE(C9, D9, E9)</f>
-        <v>38.790563766300004</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A2:A9"/>
+  <mergeCells count="8">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="H2:H11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>